<commit_message>
Fellowship Poster and Abstract
</commit_message>
<xml_diff>
--- a/Stims/Materials.xlsx
+++ b/Stims/Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel\Documents\Social.Influence_Speech.Perception\SI.SP\Stims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82150F06-FEB5-4ECE-9C41-9DB3F425F288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67749914-11E3-441B-846A-CCED653ACA2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{BE94E350-9BA2-40B7-B37A-9E00105A1A32}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="82">
   <si>
     <t>Vacation</t>
   </si>
@@ -206,9 +206,6 @@
   </si>
   <si>
     <t xml:space="preserve">Pair each S word to one Sh word. The words within each pairing should be as distinct-sounding from their counterpart as possible. </t>
-  </si>
-  <si>
-    <t>S/Sh word pairings are used because earlier research suggests that listeners perceive an individual's production of sounds on the S-Sh continuum as specific to that talker. As a result, listeners have been found to adjust their perception of S-Sh independently across  talkers' speech, meaning it would be possible to simulate 2 distinct talkers with different production boundaries between S and Sh during the same exposure phase. This will thus allow us to simulate two talkers simultaneously and investigate the role of attention on speech perception adapation when a listener is instructed to attend to one of the talkers.</t>
   </si>
   <si>
     <r>
@@ -570,12 +567,21 @@
   <si>
     <t>Peninsula</t>
   </si>
+  <si>
+    <t>(Talker 1)</t>
+  </si>
+  <si>
+    <t>(Talker 2)</t>
+  </si>
+  <si>
+    <t>S/Sh word pairings are used because earlier research suggests that listeners perceive an individual's production of sounds on the S-Sh continuum as specific to that talker. As a result, listeners have been found to adjust their perception of S-Sh independently across  talkers' speech, meaning it would be possible to simulate 2 distinct talkers with different production boundaries between S and Sh during the same exposure phase. This will thus allow us to simulate two talkers simultaneously and investigate the role of attention on speech perception adaptation when a listener is instructed to attend to one of the talkers.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -605,6 +611,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <color theme="1"/>
+      <name val="Sylfaen"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Sylfaen"/>
       <family val="1"/>
@@ -1268,7 +1281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1524,9 +1537,6 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1539,33 +1549,15 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1580,6 +1572,36 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1593,9 +1615,6 @@
     <xf numFmtId="0" fontId="1" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1614,31 +1633,34 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="180"/>
     </xf>
   </cellXfs>
@@ -1649,6 +1671,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFBE5F"/>
       <color rgb="FFFFE5FB"/>
       <color rgb="FFFFDDFA"/>
       <color rgb="FFECF1DB"/>
@@ -1658,7 +1681,6 @@
       <color rgb="FFBFE4FD"/>
       <color rgb="FFFFC1F6"/>
       <color rgb="FFFFC5F7"/>
-      <color rgb="FFEFE5FF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1971,8 +1993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26893740-08BF-46AB-82EB-D9B605E89688}">
   <dimension ref="B2:AG41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="110" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y3" sqref="Y3:Y26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1989,21 +2011,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:33" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="U2" s="135" t="s">
+      <c r="U2" s="113" t="s">
         <v>51</v>
       </c>
-      <c r="V2" s="136"/>
-      <c r="W2" s="136"/>
-      <c r="Z2" s="135" t="s">
+      <c r="V2" s="114"/>
+      <c r="W2" s="114"/>
+      <c r="Z2" s="113" t="s">
         <v>48</v>
       </c>
-      <c r="AA2" s="135"/>
-      <c r="AB2" s="135"/>
-      <c r="AC2" s="135"/>
-      <c r="AD2" s="135"/>
-      <c r="AE2" s="135"/>
-      <c r="AF2" s="135"/>
-      <c r="AG2" s="135"/>
+      <c r="AA2" s="113"/>
+      <c r="AB2" s="113"/>
+      <c r="AC2" s="113"/>
+      <c r="AD2" s="113"/>
+      <c r="AE2" s="113"/>
+      <c r="AF2" s="113"/>
+      <c r="AG2" s="113"/>
     </row>
     <row r="3" spans="2:33" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="36" t="s">
@@ -2012,11 +2034,11 @@
       <c r="C3" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="131" t="s">
+      <c r="D3" s="119" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="132"/>
-      <c r="F3" s="132"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="120"/>
       <c r="G3" s="94"/>
       <c r="H3" s="8" t="s">
         <v>37</v>
@@ -2024,21 +2046,21 @@
       <c r="I3" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="131" t="s">
+      <c r="J3" s="119" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="132"/>
-      <c r="L3" s="132"/>
+      <c r="K3" s="120"/>
+      <c r="L3" s="120"/>
       <c r="M3" s="14"/>
-      <c r="N3" s="135" t="s">
+      <c r="N3" s="113" t="s">
         <v>44</v>
       </c>
-      <c r="O3" s="136"/>
-      <c r="Q3" s="137" t="s">
+      <c r="O3" s="114"/>
+      <c r="Q3" s="115" t="s">
         <v>45</v>
       </c>
-      <c r="R3" s="137"/>
-      <c r="S3" s="138" t="s">
+      <c r="R3" s="115"/>
+      <c r="S3" s="141" t="s">
         <v>37</v>
       </c>
       <c r="T3" s="47"/>
@@ -2046,7 +2068,7 @@
       <c r="V3" s="46"/>
       <c r="W3" s="48"/>
       <c r="X3" s="47"/>
-      <c r="Y3" s="139" t="s">
+      <c r="Y3" s="142" t="s">
         <v>38</v>
       </c>
       <c r="Z3" s="92"/>
@@ -2054,56 +2076,56 @@
       <c r="AB3" s="92"/>
       <c r="AC3" s="92"/>
       <c r="AD3" s="92"/>
-      <c r="AE3" s="124" t="s">
-        <v>69</v>
-      </c>
-      <c r="AF3" s="124"/>
-      <c r="AG3" s="124"/>
+      <c r="AE3" s="117" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF3" s="117"/>
+      <c r="AG3" s="117"/>
     </row>
     <row r="4" spans="2:33" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="131"/>
-      <c r="E4" s="132"/>
-      <c r="F4" s="132"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="120"/>
+      <c r="F4" s="120"/>
       <c r="G4" s="94"/>
       <c r="H4" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="131"/>
-      <c r="K4" s="132"/>
-      <c r="L4" s="132"/>
+      <c r="J4" s="119"/>
+      <c r="K4" s="120"/>
+      <c r="L4" s="120"/>
       <c r="M4" s="14"/>
-      <c r="N4" s="104" t="s">
+      <c r="N4" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="O4" s="103" t="s">
+      <c r="O4" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="Q4" s="102" t="s">
+      <c r="Q4" s="101" t="s">
         <v>37</v>
       </c>
-      <c r="R4" s="105" t="s">
+      <c r="R4" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="S4" s="138"/>
+      <c r="S4" s="116"/>
       <c r="T4" s="63"/>
       <c r="U4" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="V4" s="45"/>
       <c r="W4" s="15" t="s">
         <v>40</v>
       </c>
       <c r="X4" s="59"/>
-      <c r="Y4" s="139"/>
+      <c r="Y4" s="118"/>
       <c r="Z4" s="68" t="s">
         <v>37</v>
       </c>
@@ -2112,9 +2134,9 @@
       </c>
       <c r="AB4" s="70"/>
       <c r="AC4" s="71"/>
-      <c r="AE4" s="124"/>
-      <c r="AF4" s="124"/>
-      <c r="AG4" s="124"/>
+      <c r="AE4" s="117"/>
+      <c r="AF4" s="117"/>
+      <c r="AG4" s="117"/>
     </row>
     <row r="5" spans="2:33" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="33" t="s">
@@ -2123,11 +2145,11 @@
       <c r="C5" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="131" t="s">
+      <c r="D5" s="119" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="132"/>
-      <c r="F5" s="132"/>
+      <c r="E5" s="120"/>
+      <c r="F5" s="120"/>
       <c r="G5" s="94"/>
       <c r="H5" s="5" t="s">
         <v>17</v>
@@ -2135,46 +2157,46 @@
       <c r="I5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="131"/>
-      <c r="K5" s="132"/>
-      <c r="L5" s="132"/>
+      <c r="J5" s="119"/>
+      <c r="K5" s="120"/>
+      <c r="L5" s="120"/>
       <c r="M5" s="14"/>
-      <c r="N5" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="O5" s="101" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q5" s="106" t="s">
-        <v>63</v>
-      </c>
-      <c r="R5" s="107" t="s">
-        <v>62</v>
-      </c>
-      <c r="S5" s="138"/>
+      <c r="N5" s="133" t="s">
+        <v>79</v>
+      </c>
+      <c r="O5" s="134" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q5" s="135" t="s">
+        <v>80</v>
+      </c>
+      <c r="R5" s="136" t="s">
+        <v>79</v>
+      </c>
+      <c r="S5" s="116"/>
       <c r="T5" s="64"/>
       <c r="U5" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="V5" s="108" t="s">
-        <v>72</v>
+      <c r="V5" s="105" t="s">
+        <v>71</v>
       </c>
       <c r="W5" s="21" t="s">
         <v>33</v>
       </c>
       <c r="X5" s="60"/>
-      <c r="Y5" s="139"/>
+      <c r="Y5" s="118"/>
       <c r="Z5" s="72" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AA5" s="73" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AB5" s="74"/>
       <c r="AC5" s="75"/>
-      <c r="AE5" s="124"/>
-      <c r="AF5" s="124"/>
-      <c r="AG5" s="124"/>
+      <c r="AE5" s="117"/>
+      <c r="AF5" s="117"/>
+      <c r="AG5" s="117"/>
     </row>
     <row r="6" spans="2:33" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="39" t="s">
@@ -2193,12 +2215,12 @@
       <c r="I6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="131"/>
-      <c r="K6" s="132"/>
-      <c r="L6" s="132"/>
+      <c r="J6" s="119"/>
+      <c r="K6" s="120"/>
+      <c r="L6" s="120"/>
       <c r="M6" s="14"/>
       <c r="N6" s="99" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O6" s="100" t="s">
         <v>23</v>
@@ -2209,30 +2231,30 @@
       <c r="R6" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="S6" s="138"/>
+      <c r="S6" s="116"/>
       <c r="T6" s="64"/>
       <c r="U6" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="V6" s="108" t="s">
-        <v>73</v>
+      <c r="V6" s="105" t="s">
+        <v>72</v>
       </c>
       <c r="W6" s="17" t="s">
         <v>31</v>
       </c>
       <c r="X6" s="60"/>
-      <c r="Y6" s="139"/>
+      <c r="Y6" s="118"/>
       <c r="Z6" s="76"/>
       <c r="AA6" s="77"/>
       <c r="AB6" s="78" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AC6" s="79" t="s">
-        <v>71</v>
-      </c>
-      <c r="AE6" s="124"/>
-      <c r="AF6" s="124"/>
-      <c r="AG6" s="124"/>
+        <v>70</v>
+      </c>
+      <c r="AE6" s="117"/>
+      <c r="AF6" s="117"/>
+      <c r="AG6" s="117"/>
     </row>
     <row r="7" spans="2:33" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="33" t="s">
@@ -2241,11 +2263,11 @@
       <c r="C7" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="131" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="132"/>
-      <c r="F7" s="132"/>
+      <c r="D7" s="119" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="120"/>
+      <c r="F7" s="120"/>
       <c r="G7" s="94"/>
       <c r="H7" s="5" t="s">
         <v>15</v>
@@ -2253,9 +2275,9 @@
       <c r="I7" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="131"/>
-      <c r="K7" s="132"/>
-      <c r="L7" s="132"/>
+      <c r="J7" s="119"/>
+      <c r="K7" s="120"/>
+      <c r="L7" s="120"/>
       <c r="M7" s="14"/>
       <c r="N7" s="28" t="s">
         <v>8</v>
@@ -2269,19 +2291,19 @@
       <c r="R7" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="S7" s="138"/>
+      <c r="S7" s="116"/>
       <c r="T7" s="64"/>
       <c r="U7" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="V7" s="108" t="s">
-        <v>76</v>
+      <c r="V7" s="105" t="s">
+        <v>75</v>
       </c>
       <c r="W7" s="21" t="s">
         <v>27</v>
       </c>
       <c r="X7" s="60"/>
-      <c r="Y7" s="139"/>
+      <c r="Y7" s="118"/>
       <c r="Z7" s="80"/>
       <c r="AA7" s="81"/>
       <c r="AB7" s="82" t="s">
@@ -2290,9 +2312,9 @@
       <c r="AC7" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="AE7" s="124"/>
-      <c r="AF7" s="124"/>
-      <c r="AG7" s="124"/>
+      <c r="AE7" s="117"/>
+      <c r="AF7" s="117"/>
+      <c r="AG7" s="117"/>
     </row>
     <row r="8" spans="2:33" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="39" t="s">
@@ -2301,21 +2323,21 @@
       <c r="C8" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="131"/>
-      <c r="E8" s="132"/>
-      <c r="F8" s="132"/>
+      <c r="D8" s="119"/>
+      <c r="E8" s="120"/>
+      <c r="F8" s="120"/>
       <c r="G8" s="67"/>
       <c r="H8" s="11" t="s">
         <v>14</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="J8" s="133" t="s">
+        <v>78</v>
+      </c>
+      <c r="J8" s="121" t="s">
         <v>43</v>
       </c>
-      <c r="K8" s="134"/>
-      <c r="L8" s="134"/>
+      <c r="K8" s="122"/>
+      <c r="L8" s="122"/>
       <c r="M8" s="2"/>
       <c r="N8" s="24" t="s">
         <v>16</v>
@@ -2329,26 +2351,26 @@
       <c r="R8" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="S8" s="138"/>
+      <c r="S8" s="116"/>
       <c r="T8" s="64"/>
       <c r="U8" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="V8" s="108" t="s">
-        <v>77</v>
+      <c r="V8" s="105" t="s">
+        <v>76</v>
       </c>
       <c r="W8" s="17" t="s">
         <v>20</v>
       </c>
       <c r="X8" s="60"/>
-      <c r="Y8" s="139"/>
+      <c r="Y8" s="118"/>
       <c r="Z8" s="3"/>
       <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
       <c r="AC8" s="3"/>
-      <c r="AE8" s="124"/>
-      <c r="AF8" s="124"/>
-      <c r="AG8" s="124"/>
+      <c r="AE8" s="117"/>
+      <c r="AF8" s="117"/>
+      <c r="AG8" s="117"/>
     </row>
     <row r="9" spans="2:33" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="33" t="s">
@@ -2357,9 +2379,9 @@
       <c r="C9" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="131"/>
-      <c r="E9" s="132"/>
-      <c r="F9" s="132"/>
+      <c r="D9" s="119"/>
+      <c r="E9" s="120"/>
+      <c r="F9" s="120"/>
       <c r="G9" s="94"/>
       <c r="H9" s="5" t="s">
         <v>18</v>
@@ -2379,19 +2401,19 @@
       <c r="R9" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="S9" s="138"/>
+      <c r="S9" s="116"/>
       <c r="T9" s="64"/>
       <c r="U9" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="V9" s="108" t="s">
-        <v>75</v>
+      <c r="V9" s="105" t="s">
+        <v>74</v>
       </c>
       <c r="W9" s="21" t="s">
         <v>21</v>
       </c>
       <c r="X9" s="60"/>
-      <c r="Y9" s="139"/>
+      <c r="Y9" s="118"/>
       <c r="Z9" s="68"/>
       <c r="AA9" s="69"/>
       <c r="AB9" s="70" t="s">
@@ -2400,9 +2422,9 @@
       <c r="AC9" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="AE9" s="124"/>
-      <c r="AF9" s="124"/>
-      <c r="AG9" s="124"/>
+      <c r="AE9" s="117"/>
+      <c r="AF9" s="117"/>
+      <c r="AG9" s="117"/>
     </row>
     <row r="10" spans="2:33" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="39" t="s">
@@ -2411,9 +2433,9 @@
       <c r="C10" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="131"/>
-      <c r="E10" s="132"/>
-      <c r="F10" s="132"/>
+      <c r="D10" s="119"/>
+      <c r="E10" s="120"/>
+      <c r="F10" s="120"/>
       <c r="G10" s="94"/>
       <c r="H10" s="11" t="s">
         <v>13</v>
@@ -2421,16 +2443,16 @@
       <c r="I10" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J10" s="131" t="s">
-        <v>58</v>
-      </c>
-      <c r="K10" s="132"/>
-      <c r="L10" s="132"/>
+      <c r="J10" s="119" t="s">
+        <v>57</v>
+      </c>
+      <c r="K10" s="120"/>
+      <c r="L10" s="120"/>
       <c r="N10" s="24" t="s">
         <v>14</v>
       </c>
       <c r="O10" s="30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q10" s="22" t="s">
         <v>5</v>
@@ -2438,30 +2460,30 @@
       <c r="R10" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="S10" s="138"/>
+      <c r="S10" s="116"/>
       <c r="T10" s="64"/>
       <c r="U10" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="V10" s="108" t="s">
-        <v>74</v>
+      <c r="V10" s="105" t="s">
+        <v>73</v>
       </c>
       <c r="W10" s="17" t="s">
         <v>29</v>
       </c>
       <c r="X10" s="60"/>
-      <c r="Y10" s="139"/>
+      <c r="Y10" s="118"/>
       <c r="Z10" s="72"/>
       <c r="AA10" s="73"/>
       <c r="AB10" s="74" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AC10" s="75" t="s">
-        <v>71</v>
-      </c>
-      <c r="AE10" s="124"/>
-      <c r="AF10" s="124"/>
-      <c r="AG10" s="124"/>
+        <v>70</v>
+      </c>
+      <c r="AE10" s="117"/>
+      <c r="AF10" s="117"/>
+      <c r="AG10" s="117"/>
     </row>
     <row r="11" spans="2:33" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="33" t="s">
@@ -2470,9 +2492,9 @@
       <c r="C11" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="131"/>
-      <c r="E11" s="132"/>
-      <c r="F11" s="132"/>
+      <c r="D11" s="119"/>
+      <c r="E11" s="120"/>
+      <c r="F11" s="120"/>
       <c r="G11" s="94"/>
       <c r="H11" s="5" t="s">
         <v>12</v>
@@ -2480,9 +2502,9 @@
       <c r="I11" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="J11" s="131"/>
-      <c r="K11" s="132"/>
-      <c r="L11" s="132"/>
+      <c r="J11" s="119"/>
+      <c r="K11" s="120"/>
+      <c r="L11" s="120"/>
       <c r="N11" s="28" t="s">
         <v>4</v>
       </c>
@@ -2495,28 +2517,28 @@
       <c r="R11" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="S11" s="138"/>
+      <c r="S11" s="116"/>
       <c r="T11" s="64"/>
       <c r="U11" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="V11" s="108"/>
+      <c r="V11" s="105"/>
       <c r="W11" s="21" t="s">
         <v>30</v>
       </c>
       <c r="X11" s="60"/>
-      <c r="Y11" s="139"/>
+      <c r="Y11" s="118"/>
       <c r="Z11" s="76" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AA11" s="77" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AB11" s="78"/>
       <c r="AC11" s="79"/>
-      <c r="AE11" s="124"/>
-      <c r="AF11" s="124"/>
-      <c r="AG11" s="124"/>
+      <c r="AE11" s="117"/>
+      <c r="AF11" s="117"/>
+      <c r="AG11" s="117"/>
     </row>
     <row r="12" spans="2:33" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="39" t="s">
@@ -2525,9 +2547,9 @@
       <c r="C12" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="131"/>
-      <c r="E12" s="132"/>
-      <c r="F12" s="132"/>
+      <c r="D12" s="119"/>
+      <c r="E12" s="120"/>
+      <c r="F12" s="120"/>
       <c r="G12" s="94"/>
       <c r="H12" s="11" t="s">
         <v>11</v>
@@ -2535,9 +2557,9 @@
       <c r="I12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="J12" s="131"/>
-      <c r="K12" s="132"/>
-      <c r="L12" s="132"/>
+      <c r="J12" s="119"/>
+      <c r="K12" s="120"/>
+      <c r="L12" s="120"/>
       <c r="N12" s="24" t="s">
         <v>13</v>
       </c>
@@ -2550,19 +2572,19 @@
       <c r="R12" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="S12" s="138"/>
+      <c r="S12" s="116"/>
       <c r="T12" s="64"/>
       <c r="U12" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="V12" s="108">
+      <c r="V12" s="105">
         <v>1</v>
       </c>
       <c r="W12" s="17" t="s">
         <v>26</v>
       </c>
       <c r="X12" s="60"/>
-      <c r="Y12" s="139"/>
+      <c r="Y12" s="118"/>
       <c r="Z12" s="80" t="s">
         <v>37</v>
       </c>
@@ -2582,9 +2604,9 @@
       <c r="C13" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="131"/>
-      <c r="E13" s="132"/>
-      <c r="F13" s="132"/>
+      <c r="D13" s="119"/>
+      <c r="E13" s="120"/>
+      <c r="F13" s="120"/>
       <c r="G13" s="94"/>
       <c r="H13" s="5" t="s">
         <v>10</v>
@@ -2592,9 +2614,9 @@
       <c r="I13" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="J13" s="131"/>
-      <c r="K13" s="132"/>
-      <c r="L13" s="132"/>
+      <c r="J13" s="119"/>
+      <c r="K13" s="120"/>
+      <c r="L13" s="120"/>
       <c r="N13" s="28" t="s">
         <v>2</v>
       </c>
@@ -2607,7 +2629,7 @@
       <c r="R13" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="S13" s="138"/>
+      <c r="S13" s="116"/>
       <c r="T13" s="64"/>
       <c r="U13" s="43" t="s">
         <v>0</v>
@@ -2617,7 +2639,7 @@
         <v>35</v>
       </c>
       <c r="X13" s="60"/>
-      <c r="Y13" s="139"/>
+      <c r="Y13" s="118"/>
       <c r="Z13" s="3"/>
       <c r="AA13" s="3"/>
       <c r="AB13" s="3"/>
@@ -2633,9 +2655,9 @@
       <c r="C14" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="131"/>
-      <c r="E14" s="132"/>
-      <c r="F14" s="132"/>
+      <c r="D14" s="119"/>
+      <c r="E14" s="120"/>
+      <c r="F14" s="120"/>
       <c r="G14" s="94"/>
       <c r="H14" s="11" t="s">
         <v>9</v>
@@ -2643,9 +2665,9 @@
       <c r="I14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="131"/>
-      <c r="K14" s="132"/>
-      <c r="L14" s="132"/>
+      <c r="J14" s="119"/>
+      <c r="K14" s="120"/>
+      <c r="L14" s="120"/>
       <c r="N14" s="24" t="s">
         <v>11</v>
       </c>
@@ -2658,13 +2680,13 @@
       <c r="R14" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="S14" s="138"/>
+      <c r="S14" s="116"/>
       <c r="T14" s="65"/>
       <c r="U14" s="58"/>
       <c r="V14" s="57"/>
       <c r="W14" s="56"/>
       <c r="X14" s="61"/>
-      <c r="Y14" s="139"/>
+      <c r="Y14" s="118"/>
       <c r="Z14" s="68" t="s">
         <v>37</v>
       </c>
@@ -2673,11 +2695,11 @@
       </c>
       <c r="AB14" s="85"/>
       <c r="AC14" s="71"/>
-      <c r="AE14" s="124" t="s">
-        <v>70</v>
-      </c>
-      <c r="AF14" s="124"/>
-      <c r="AG14" s="124"/>
+      <c r="AE14" s="117" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF14" s="117"/>
+      <c r="AG14" s="117"/>
     </row>
     <row r="15" spans="2:33" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="33" t="s">
@@ -2686,9 +2708,9 @@
       <c r="C15" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="131"/>
-      <c r="E15" s="132"/>
-      <c r="F15" s="132"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="120"/>
+      <c r="F15" s="120"/>
       <c r="G15" s="94"/>
       <c r="H15" s="5" t="s">
         <v>8</v>
@@ -2696,9 +2718,9 @@
       <c r="I15" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="131"/>
-      <c r="K15" s="132"/>
-      <c r="L15" s="132"/>
+      <c r="J15" s="119"/>
+      <c r="K15" s="120"/>
+      <c r="L15" s="120"/>
       <c r="N15" s="29" t="s">
         <v>0</v>
       </c>
@@ -2711,24 +2733,24 @@
       <c r="R15" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="S15" s="138"/>
+      <c r="S15" s="116"/>
       <c r="T15" s="64"/>
       <c r="U15" s="55"/>
       <c r="V15" s="53"/>
       <c r="W15" s="54"/>
       <c r="X15" s="60"/>
-      <c r="Y15" s="139"/>
+      <c r="Y15" s="118"/>
       <c r="Z15" s="72" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AA15" s="86" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AB15" s="77"/>
       <c r="AC15" s="75"/>
-      <c r="AE15" s="124"/>
-      <c r="AF15" s="124"/>
-      <c r="AG15" s="124"/>
+      <c r="AE15" s="117"/>
+      <c r="AF15" s="117"/>
+      <c r="AG15" s="117"/>
     </row>
     <row r="16" spans="2:33" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="39" t="s">
@@ -2737,9 +2759,9 @@
       <c r="C16" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="131"/>
-      <c r="E16" s="132"/>
-      <c r="F16" s="132"/>
+      <c r="D16" s="119"/>
+      <c r="E16" s="120"/>
+      <c r="F16" s="120"/>
       <c r="G16" s="94"/>
       <c r="H16" s="11" t="s">
         <v>7</v>
@@ -2747,10 +2769,10 @@
       <c r="I16" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="J16" s="131"/>
-      <c r="K16" s="132"/>
-      <c r="L16" s="132"/>
-      <c r="S16" s="138"/>
+      <c r="J16" s="119"/>
+      <c r="K16" s="120"/>
+      <c r="L16" s="120"/>
+      <c r="S16" s="116"/>
       <c r="T16" s="64"/>
       <c r="U16" s="44" t="s">
         <v>9</v>
@@ -2760,18 +2782,18 @@
         <v>23</v>
       </c>
       <c r="X16" s="60"/>
-      <c r="Y16" s="139"/>
+      <c r="Y16" s="118"/>
       <c r="Z16" s="76"/>
       <c r="AA16" s="74"/>
       <c r="AB16" s="87" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AC16" s="79" t="s">
-        <v>71</v>
-      </c>
-      <c r="AE16" s="124"/>
-      <c r="AF16" s="124"/>
-      <c r="AG16" s="124"/>
+        <v>70</v>
+      </c>
+      <c r="AE16" s="117"/>
+      <c r="AF16" s="117"/>
+      <c r="AG16" s="117"/>
     </row>
     <row r="17" spans="2:33" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B17" s="33" t="s">
@@ -2780,9 +2802,9 @@
       <c r="C17" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="131"/>
-      <c r="E17" s="132"/>
-      <c r="F17" s="132"/>
+      <c r="D17" s="119"/>
+      <c r="E17" s="120"/>
+      <c r="F17" s="120"/>
       <c r="G17" s="94"/>
       <c r="H17" s="5" t="s">
         <v>6</v>
@@ -2790,29 +2812,29 @@
       <c r="I17" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="J17" s="131"/>
-      <c r="K17" s="132"/>
-      <c r="L17" s="132"/>
-      <c r="N17" s="124" t="s">
-        <v>68</v>
-      </c>
-      <c r="O17" s="124"/>
-      <c r="P17" s="124"/>
-      <c r="Q17" s="124"/>
-      <c r="R17" s="124"/>
-      <c r="S17" s="138"/>
+      <c r="J17" s="119"/>
+      <c r="K17" s="120"/>
+      <c r="L17" s="120"/>
+      <c r="N17" s="117" t="s">
+        <v>67</v>
+      </c>
+      <c r="O17" s="117"/>
+      <c r="P17" s="117"/>
+      <c r="Q17" s="117"/>
+      <c r="R17" s="117"/>
+      <c r="S17" s="116"/>
       <c r="T17" s="64"/>
       <c r="U17" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="V17" s="109" t="s">
-        <v>72</v>
+      <c r="V17" s="106" t="s">
+        <v>71</v>
       </c>
       <c r="W17" s="26" t="s">
         <v>24</v>
       </c>
       <c r="X17" s="60"/>
-      <c r="Y17" s="139"/>
+      <c r="Y17" s="118"/>
       <c r="Z17" s="80"/>
       <c r="AA17" s="88"/>
       <c r="AB17" s="89" t="s">
@@ -2821,20 +2843,20 @@
       <c r="AC17" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="AE17" s="124"/>
-      <c r="AF17" s="124"/>
-      <c r="AG17" s="124"/>
+      <c r="AE17" s="117"/>
+      <c r="AF17" s="117"/>
+      <c r="AG17" s="117"/>
     </row>
     <row r="18" spans="2:33" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="39" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" s="131"/>
-      <c r="E18" s="132"/>
-      <c r="F18" s="132"/>
+        <v>78</v>
+      </c>
+      <c r="D18" s="119"/>
+      <c r="E18" s="120"/>
+      <c r="F18" s="120"/>
       <c r="G18" s="94"/>
       <c r="H18" s="11" t="s">
         <v>5</v>
@@ -2842,34 +2864,34 @@
       <c r="I18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J18" s="131"/>
-      <c r="K18" s="132"/>
-      <c r="L18" s="132"/>
-      <c r="N18" s="124"/>
-      <c r="O18" s="124"/>
-      <c r="P18" s="124"/>
-      <c r="Q18" s="124"/>
-      <c r="R18" s="124"/>
-      <c r="S18" s="138"/>
+      <c r="J18" s="119"/>
+      <c r="K18" s="120"/>
+      <c r="L18" s="120"/>
+      <c r="N18" s="117"/>
+      <c r="O18" s="117"/>
+      <c r="P18" s="117"/>
+      <c r="Q18" s="117"/>
+      <c r="R18" s="117"/>
+      <c r="S18" s="116"/>
       <c r="T18" s="64"/>
       <c r="U18" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="V18" s="109" t="s">
-        <v>73</v>
+      <c r="V18" s="106" t="s">
+        <v>72</v>
       </c>
       <c r="W18" s="30" t="s">
         <v>25</v>
       </c>
       <c r="X18" s="60"/>
-      <c r="Y18" s="139"/>
+      <c r="Y18" s="118"/>
       <c r="Z18" s="3"/>
       <c r="AA18" s="3"/>
       <c r="AB18" s="3"/>
       <c r="AC18" s="3"/>
-      <c r="AE18" s="124"/>
-      <c r="AF18" s="124"/>
-      <c r="AG18" s="124"/>
+      <c r="AE18" s="117"/>
+      <c r="AF18" s="117"/>
+      <c r="AG18" s="117"/>
     </row>
     <row r="19" spans="2:33" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="33" t="s">
@@ -2878,9 +2900,9 @@
       <c r="C19" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="131"/>
-      <c r="E19" s="132"/>
-      <c r="F19" s="132"/>
+      <c r="D19" s="119"/>
+      <c r="E19" s="120"/>
+      <c r="F19" s="120"/>
       <c r="G19" s="94"/>
       <c r="H19" s="5" t="s">
         <v>4</v>
@@ -2888,27 +2910,27 @@
       <c r="I19" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="J19" s="131"/>
-      <c r="K19" s="132"/>
-      <c r="L19" s="132"/>
-      <c r="N19" s="124"/>
-      <c r="O19" s="124"/>
-      <c r="P19" s="124"/>
-      <c r="Q19" s="124"/>
-      <c r="R19" s="124"/>
-      <c r="S19" s="138"/>
+      <c r="J19" s="119"/>
+      <c r="K19" s="120"/>
+      <c r="L19" s="120"/>
+      <c r="N19" s="117"/>
+      <c r="O19" s="117"/>
+      <c r="P19" s="117"/>
+      <c r="Q19" s="117"/>
+      <c r="R19" s="117"/>
+      <c r="S19" s="116"/>
       <c r="T19" s="64"/>
       <c r="U19" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="V19" s="109" t="s">
-        <v>76</v>
+      <c r="V19" s="106" t="s">
+        <v>75</v>
       </c>
       <c r="W19" s="26" t="s">
         <v>41</v>
       </c>
       <c r="X19" s="60"/>
-      <c r="Y19" s="139"/>
+      <c r="Y19" s="118"/>
       <c r="Z19" s="68"/>
       <c r="AA19" s="84"/>
       <c r="AB19" s="85" t="s">
@@ -2925,9 +2947,9 @@
       <c r="C20" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="131"/>
-      <c r="E20" s="132"/>
-      <c r="F20" s="132"/>
+      <c r="D20" s="119"/>
+      <c r="E20" s="120"/>
+      <c r="F20" s="120"/>
       <c r="G20" s="94"/>
       <c r="H20" s="11" t="s">
         <v>3</v>
@@ -2935,40 +2957,40 @@
       <c r="I20" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="J20" s="131"/>
-      <c r="K20" s="132"/>
-      <c r="L20" s="132"/>
-      <c r="N20" s="124"/>
-      <c r="O20" s="124"/>
-      <c r="P20" s="124"/>
-      <c r="Q20" s="124"/>
-      <c r="R20" s="124"/>
-      <c r="S20" s="138"/>
+      <c r="J20" s="119"/>
+      <c r="K20" s="120"/>
+      <c r="L20" s="120"/>
+      <c r="N20" s="117"/>
+      <c r="O20" s="117"/>
+      <c r="P20" s="117"/>
+      <c r="Q20" s="117"/>
+      <c r="R20" s="117"/>
+      <c r="S20" s="116"/>
       <c r="T20" s="64"/>
       <c r="U20" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="V20" s="109" t="s">
-        <v>77</v>
+      <c r="V20" s="106" t="s">
+        <v>76</v>
       </c>
       <c r="W20" s="30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="X20" s="60"/>
-      <c r="Y20" s="139"/>
+      <c r="Y20" s="118"/>
       <c r="Z20" s="72"/>
       <c r="AA20" s="86"/>
       <c r="AB20" s="77" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AC20" s="75" t="s">
-        <v>71</v>
-      </c>
-      <c r="AE20" s="124" t="s">
-        <v>67</v>
-      </c>
-      <c r="AF20" s="124"/>
-      <c r="AG20" s="124"/>
+        <v>70</v>
+      </c>
+      <c r="AE20" s="117" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF20" s="117"/>
+      <c r="AG20" s="117"/>
     </row>
     <row r="21" spans="2:33" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="33" t="s">
@@ -2977,9 +2999,9 @@
       <c r="C21" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="131"/>
-      <c r="E21" s="132"/>
-      <c r="F21" s="132"/>
+      <c r="D21" s="119"/>
+      <c r="E21" s="120"/>
+      <c r="F21" s="120"/>
       <c r="G21" s="94"/>
       <c r="H21" s="5" t="s">
         <v>2</v>
@@ -2987,32 +3009,32 @@
       <c r="I21" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="J21" s="131"/>
-      <c r="K21" s="132"/>
-      <c r="L21" s="132"/>
-      <c r="N21" s="124"/>
-      <c r="O21" s="124"/>
-      <c r="P21" s="124"/>
-      <c r="Q21" s="124"/>
-      <c r="R21" s="124"/>
-      <c r="S21" s="138"/>
+      <c r="J21" s="119"/>
+      <c r="K21" s="120"/>
+      <c r="L21" s="120"/>
+      <c r="N21" s="117"/>
+      <c r="O21" s="117"/>
+      <c r="P21" s="117"/>
+      <c r="Q21" s="117"/>
+      <c r="R21" s="117"/>
+      <c r="S21" s="116"/>
       <c r="T21" s="64"/>
       <c r="U21" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="V21" s="109" t="s">
-        <v>75</v>
+      <c r="V21" s="106" t="s">
+        <v>74</v>
       </c>
       <c r="W21" s="26" t="s">
         <v>28</v>
       </c>
       <c r="X21" s="60"/>
-      <c r="Y21" s="139"/>
+      <c r="Y21" s="118"/>
       <c r="Z21" s="76" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AA21" s="74" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AB21" s="87"/>
       <c r="AC21" s="79"/>
@@ -3027,9 +3049,9 @@
       <c r="C22" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="131"/>
-      <c r="E22" s="132"/>
-      <c r="F22" s="132"/>
+      <c r="D22" s="119"/>
+      <c r="E22" s="120"/>
+      <c r="F22" s="120"/>
       <c r="G22" s="94"/>
       <c r="H22" s="11" t="s">
         <v>1</v>
@@ -3037,29 +3059,29 @@
       <c r="I22" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J22" s="131"/>
-      <c r="K22" s="132"/>
-      <c r="L22" s="132"/>
-      <c r="N22" s="136" t="s">
+      <c r="J22" s="119"/>
+      <c r="K22" s="120"/>
+      <c r="L22" s="120"/>
+      <c r="N22" s="114" t="s">
         <v>46</v>
       </c>
-      <c r="O22" s="136"/>
-      <c r="P22" s="136"/>
-      <c r="Q22" s="136"/>
-      <c r="R22" s="136"/>
-      <c r="S22" s="138"/>
+      <c r="O22" s="114"/>
+      <c r="P22" s="114"/>
+      <c r="Q22" s="114"/>
+      <c r="R22" s="114"/>
+      <c r="S22" s="116"/>
       <c r="T22" s="64"/>
       <c r="U22" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="V22" s="109" t="s">
-        <v>74</v>
+      <c r="V22" s="106" t="s">
+        <v>73</v>
       </c>
       <c r="W22" s="30" t="s">
         <v>36</v>
       </c>
       <c r="X22" s="60"/>
-      <c r="Y22" s="139"/>
+      <c r="Y22" s="118"/>
       <c r="Z22" s="80" t="s">
         <v>37</v>
       </c>
@@ -3068,10 +3090,10 @@
       </c>
       <c r="AB22" s="89"/>
       <c r="AC22" s="83"/>
-      <c r="AE22" s="124" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF22" s="124"/>
+      <c r="AE22" s="117" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF22" s="117"/>
       <c r="AG22" s="42" t="s">
         <v>47</v>
       </c>
@@ -3083,9 +3105,9 @@
       <c r="C23" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="131"/>
-      <c r="E23" s="132"/>
-      <c r="F23" s="132"/>
+      <c r="D23" s="119"/>
+      <c r="E23" s="120"/>
+      <c r="F23" s="120"/>
       <c r="G23" s="94"/>
       <c r="H23" s="7" t="s">
         <v>0</v>
@@ -3093,29 +3115,29 @@
       <c r="I23" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J23" s="131"/>
-      <c r="K23" s="132"/>
-      <c r="L23" s="132"/>
-      <c r="S23" s="138"/>
+      <c r="J23" s="119"/>
+      <c r="K23" s="120"/>
+      <c r="L23" s="120"/>
+      <c r="S23" s="116"/>
       <c r="T23" s="64"/>
       <c r="U23" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="V23" s="109"/>
+      <c r="V23" s="106"/>
       <c r="W23" s="26" t="s">
         <v>34</v>
       </c>
       <c r="X23" s="60"/>
-      <c r="Y23" s="139"/>
+      <c r="Y23" s="118"/>
       <c r="Z23" s="90"/>
       <c r="AA23" s="90"/>
       <c r="AB23" s="90"/>
       <c r="AC23" s="90"/>
       <c r="AD23" s="90"/>
-      <c r="AE23" s="124" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF23" s="124"/>
+      <c r="AE23" s="117" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF23" s="117"/>
       <c r="AG23" s="42" t="s">
         <v>47</v>
       </c>
@@ -3127,36 +3149,36 @@
       <c r="N24" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="O24" s="125" t="s">
+      <c r="O24" s="127" t="s">
         <v>54</v>
       </c>
-      <c r="P24" s="127"/>
-      <c r="Q24" s="125" t="s">
+      <c r="P24" s="129"/>
+      <c r="Q24" s="127" t="s">
         <v>55</v>
       </c>
-      <c r="R24" s="126"/>
-      <c r="S24" s="138"/>
+      <c r="R24" s="128"/>
+      <c r="S24" s="116"/>
       <c r="T24" s="64"/>
       <c r="U24" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="V24" s="109">
+      <c r="V24" s="106">
         <v>2</v>
       </c>
       <c r="W24" s="30" t="s">
         <v>32</v>
       </c>
       <c r="X24" s="60"/>
-      <c r="Y24" s="139"/>
+      <c r="Y24" s="118"/>
       <c r="Z24" s="90"/>
       <c r="AA24" s="90"/>
       <c r="AB24" s="90"/>
       <c r="AC24" s="90"/>
       <c r="AD24" s="90"/>
-      <c r="AE24" s="124" t="s">
-        <v>66</v>
-      </c>
-      <c r="AF24" s="124"/>
+      <c r="AE24" s="117" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF24" s="117"/>
       <c r="AG24" s="42" t="s">
         <v>47</v>
       </c>
@@ -3173,17 +3195,17 @@
       <c r="K25" s="98"/>
       <c r="L25" s="98"/>
       <c r="N25" s="95" t="s">
-        <v>59</v>
-      </c>
-      <c r="O25" s="128">
+        <v>58</v>
+      </c>
+      <c r="O25" s="130">
         <v>0.8</v>
       </c>
-      <c r="P25" s="129"/>
-      <c r="Q25" s="128">
+      <c r="P25" s="131"/>
+      <c r="Q25" s="130">
         <v>100</v>
       </c>
-      <c r="R25" s="130"/>
-      <c r="S25" s="138"/>
+      <c r="R25" s="132"/>
+      <c r="S25" s="116"/>
       <c r="T25" s="66"/>
       <c r="U25" s="19" t="s">
         <v>10</v>
@@ -3193,7 +3215,7 @@
         <v>19</v>
       </c>
       <c r="X25" s="62"/>
-      <c r="Y25" s="139"/>
+      <c r="Y25" s="118"/>
       <c r="Z25" s="90"/>
       <c r="AA25" s="90"/>
       <c r="AB25" s="90"/>
@@ -3215,23 +3237,23 @@
       <c r="K26" s="98"/>
       <c r="L26" s="98"/>
       <c r="N26" s="96" t="s">
-        <v>60</v>
-      </c>
-      <c r="O26" s="120">
+        <v>59</v>
+      </c>
+      <c r="O26" s="123">
         <v>1</v>
       </c>
-      <c r="P26" s="121"/>
-      <c r="Q26" s="120">
+      <c r="P26" s="124"/>
+      <c r="Q26" s="123">
         <v>180</v>
       </c>
-      <c r="R26" s="123"/>
-      <c r="S26" s="138"/>
+      <c r="R26" s="126"/>
+      <c r="S26" s="116"/>
       <c r="T26" s="47"/>
       <c r="U26" s="50"/>
       <c r="V26" s="51"/>
       <c r="W26" s="52"/>
       <c r="X26" s="47"/>
-      <c r="Y26" s="139"/>
+      <c r="Y26" s="118"/>
       <c r="Z26" s="91"/>
       <c r="AA26" s="91"/>
       <c r="AB26" s="91"/>
@@ -3252,18 +3274,18 @@
       <c r="J27" s="98"/>
       <c r="K27" s="98"/>
       <c r="L27" s="98"/>
-      <c r="N27" s="122" t="s">
-        <v>61</v>
-      </c>
-      <c r="O27" s="122"/>
-      <c r="P27" s="122"/>
-      <c r="Q27" s="122"/>
-      <c r="R27" s="122"/>
-      <c r="U27" s="135" t="s">
+      <c r="N27" s="125" t="s">
+        <v>60</v>
+      </c>
+      <c r="O27" s="125"/>
+      <c r="P27" s="125"/>
+      <c r="Q27" s="125"/>
+      <c r="R27" s="125"/>
+      <c r="U27" s="113" t="s">
         <v>52</v>
       </c>
-      <c r="V27" s="136"/>
-      <c r="W27" s="136"/>
+      <c r="V27" s="114"/>
+      <c r="W27" s="114"/>
       <c r="Z27" s="91"/>
       <c r="AA27" s="91"/>
       <c r="AB27" s="91"/>
@@ -3279,51 +3301,51 @@
       <c r="AG28" s="91"/>
     </row>
     <row r="29" spans="2:33" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N29" s="135" t="s">
+      <c r="N29" s="113" t="s">
+        <v>61</v>
+      </c>
+      <c r="O29" s="114"/>
+      <c r="Q29" s="115" t="s">
         <v>62</v>
       </c>
-      <c r="O29" s="136"/>
-      <c r="Q29" s="137" t="s">
-        <v>63</v>
-      </c>
-      <c r="R29" s="137"/>
+      <c r="R29" s="115"/>
     </row>
     <row r="30" spans="2:33" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="N30" s="115" t="s">
+      <c r="N30" s="108" t="s">
         <v>37</v>
       </c>
-      <c r="O30" s="116" t="s">
+      <c r="O30" s="109" t="s">
         <v>38</v>
       </c>
-      <c r="Q30" s="117" t="s">
+      <c r="Q30" s="110" t="s">
         <v>37</v>
       </c>
-      <c r="R30" s="118" t="s">
+      <c r="R30" s="111" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="31" spans="2:33" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N31" s="110" t="s">
+      <c r="N31" s="138" t="s">
         <v>44</v>
       </c>
-      <c r="O31" s="111" t="s">
+      <c r="O31" s="137" t="s">
         <v>45</v>
       </c>
-      <c r="Q31" s="113" t="s">
+      <c r="Q31" s="139" t="s">
         <v>45</v>
       </c>
-      <c r="R31" s="114" t="s">
+      <c r="R31" s="140" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="32" spans="2:33" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="N32" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="O32" s="112" t="s">
+        <v>77</v>
+      </c>
+      <c r="O32" s="107" t="s">
         <v>40</v>
       </c>
-      <c r="Q32" s="119" t="s">
+      <c r="Q32" s="112" t="s">
         <v>9</v>
       </c>
       <c r="R32" s="32" t="s">
@@ -3458,6 +3480,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="N27:R27"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="AE24:AF24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="D3:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D7:F23"/>
+    <mergeCell ref="J3:L7"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="J10:L23"/>
     <mergeCell ref="N29:O29"/>
     <mergeCell ref="Q29:R29"/>
     <mergeCell ref="S3:S26"/>
@@ -3474,22 +3510,8 @@
     <mergeCell ref="AE20:AG20"/>
     <mergeCell ref="AE23:AF23"/>
     <mergeCell ref="AE22:AF22"/>
-    <mergeCell ref="D3:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D7:F23"/>
-    <mergeCell ref="J3:L7"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="J10:L23"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="N27:R27"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="AE24:AF24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="Q25:R25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New filler pair list design + File organization
</commit_message>
<xml_diff>
--- a/Stims/Materials.xlsx
+++ b/Stims/Materials.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel\Documents\Social.Influence_Speech.Perception\SI.SP\Stims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67749914-11E3-441B-846A-CCED653ACA2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CC07E6-CB4C-4E96-83B3-2123B58F6954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{BE94E350-9BA2-40B7-B37A-9E00105A1A32}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="84">
   <si>
     <t>Vacation</t>
   </si>
@@ -575,6 +575,12 @@
   </si>
   <si>
     <t>S/Sh word pairings are used because earlier research suggests that listeners perceive an individual's production of sounds on the S-Sh continuum as specific to that talker. As a result, listeners have been found to adjust their perception of S-Sh independently across  talkers' speech, meaning it would be possible to simulate 2 distinct talkers with different production boundaries between S and Sh during the same exposure phase. This will thus allow us to simulate two talkers simultaneously and investigate the role of attention on speech perception adaptation when a listener is instructed to attend to one of the talkers.</t>
+  </si>
+  <si>
+    <t>Negotiate</t>
+  </si>
+  <si>
+    <t>Rehearsal</t>
   </si>
 </sst>
 </file>
@@ -1573,6 +1579,75 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1582,85 +1657,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="180"/>
     </xf>
   </cellXfs>
@@ -1993,8 +1999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26893740-08BF-46AB-82EB-D9B605E89688}">
   <dimension ref="B2:AG41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="110" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y3" sqref="Y3:Y26"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="92" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U35" sqref="U35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2011,21 +2017,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:33" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="U2" s="113" t="s">
+      <c r="U2" s="136" t="s">
         <v>51</v>
       </c>
-      <c r="V2" s="114"/>
-      <c r="W2" s="114"/>
-      <c r="Z2" s="113" t="s">
+      <c r="V2" s="137"/>
+      <c r="W2" s="137"/>
+      <c r="Z2" s="136" t="s">
         <v>48</v>
       </c>
-      <c r="AA2" s="113"/>
-      <c r="AB2" s="113"/>
-      <c r="AC2" s="113"/>
-      <c r="AD2" s="113"/>
-      <c r="AE2" s="113"/>
-      <c r="AF2" s="113"/>
-      <c r="AG2" s="113"/>
+      <c r="AA2" s="136"/>
+      <c r="AB2" s="136"/>
+      <c r="AC2" s="136"/>
+      <c r="AD2" s="136"/>
+      <c r="AE2" s="136"/>
+      <c r="AF2" s="136"/>
+      <c r="AG2" s="136"/>
     </row>
     <row r="3" spans="2:33" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="36" t="s">
@@ -2034,11 +2040,11 @@
       <c r="C3" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="119" t="s">
+      <c r="D3" s="132" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="120"/>
-      <c r="F3" s="120"/>
+      <c r="E3" s="133"/>
+      <c r="F3" s="133"/>
       <c r="G3" s="94"/>
       <c r="H3" s="8" t="s">
         <v>37</v>
@@ -2046,21 +2052,21 @@
       <c r="I3" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="119" t="s">
+      <c r="J3" s="132" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="120"/>
-      <c r="L3" s="120"/>
+      <c r="K3" s="133"/>
+      <c r="L3" s="133"/>
       <c r="M3" s="14"/>
-      <c r="N3" s="113" t="s">
+      <c r="N3" s="136" t="s">
         <v>44</v>
       </c>
-      <c r="O3" s="114"/>
-      <c r="Q3" s="115" t="s">
+      <c r="O3" s="137"/>
+      <c r="Q3" s="138" t="s">
         <v>45</v>
       </c>
-      <c r="R3" s="115"/>
-      <c r="S3" s="141" t="s">
+      <c r="R3" s="138"/>
+      <c r="S3" s="139" t="s">
         <v>37</v>
       </c>
       <c r="T3" s="47"/>
@@ -2068,7 +2074,7 @@
       <c r="V3" s="46"/>
       <c r="W3" s="48"/>
       <c r="X3" s="47"/>
-      <c r="Y3" s="142" t="s">
+      <c r="Y3" s="141" t="s">
         <v>38</v>
       </c>
       <c r="Z3" s="92"/>
@@ -2076,11 +2082,11 @@
       <c r="AB3" s="92"/>
       <c r="AC3" s="92"/>
       <c r="AD3" s="92"/>
-      <c r="AE3" s="117" t="s">
+      <c r="AE3" s="125" t="s">
         <v>68</v>
       </c>
-      <c r="AF3" s="117"/>
-      <c r="AG3" s="117"/>
+      <c r="AF3" s="125"/>
+      <c r="AG3" s="125"/>
     </row>
     <row r="4" spans="2:33" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="38" t="s">
@@ -2089,9 +2095,9 @@
       <c r="C4" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="119"/>
-      <c r="E4" s="120"/>
-      <c r="F4" s="120"/>
+      <c r="D4" s="132"/>
+      <c r="E4" s="133"/>
+      <c r="F4" s="133"/>
       <c r="G4" s="94"/>
       <c r="H4" s="10" t="s">
         <v>77</v>
@@ -2099,9 +2105,9 @@
       <c r="I4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="119"/>
-      <c r="K4" s="120"/>
-      <c r="L4" s="120"/>
+      <c r="J4" s="132"/>
+      <c r="K4" s="133"/>
+      <c r="L4" s="133"/>
       <c r="M4" s="14"/>
       <c r="N4" s="103" t="s">
         <v>37</v>
@@ -2115,7 +2121,7 @@
       <c r="R4" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="S4" s="116"/>
+      <c r="S4" s="140"/>
       <c r="T4" s="63"/>
       <c r="U4" s="25" t="s">
         <v>77</v>
@@ -2125,7 +2131,7 @@
         <v>40</v>
       </c>
       <c r="X4" s="59"/>
-      <c r="Y4" s="118"/>
+      <c r="Y4" s="142"/>
       <c r="Z4" s="68" t="s">
         <v>37</v>
       </c>
@@ -2134,9 +2140,9 @@
       </c>
       <c r="AB4" s="70"/>
       <c r="AC4" s="71"/>
-      <c r="AE4" s="117"/>
-      <c r="AF4" s="117"/>
-      <c r="AG4" s="117"/>
+      <c r="AE4" s="125"/>
+      <c r="AF4" s="125"/>
+      <c r="AG4" s="125"/>
     </row>
     <row r="5" spans="2:33" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="33" t="s">
@@ -2145,11 +2151,11 @@
       <c r="C5" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="119" t="s">
+      <c r="D5" s="132" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="120"/>
-      <c r="F5" s="120"/>
+      <c r="E5" s="133"/>
+      <c r="F5" s="133"/>
       <c r="G5" s="94"/>
       <c r="H5" s="5" t="s">
         <v>17</v>
@@ -2157,23 +2163,23 @@
       <c r="I5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="119"/>
-      <c r="K5" s="120"/>
-      <c r="L5" s="120"/>
+      <c r="J5" s="132"/>
+      <c r="K5" s="133"/>
+      <c r="L5" s="133"/>
       <c r="M5" s="14"/>
-      <c r="N5" s="133" t="s">
+      <c r="N5" s="113" t="s">
         <v>79</v>
       </c>
-      <c r="O5" s="134" t="s">
+      <c r="O5" s="114" t="s">
         <v>80</v>
       </c>
-      <c r="Q5" s="135" t="s">
+      <c r="Q5" s="115" t="s">
         <v>80</v>
       </c>
-      <c r="R5" s="136" t="s">
+      <c r="R5" s="116" t="s">
         <v>79</v>
       </c>
-      <c r="S5" s="116"/>
+      <c r="S5" s="140"/>
       <c r="T5" s="64"/>
       <c r="U5" s="30" t="s">
         <v>8</v>
@@ -2185,7 +2191,7 @@
         <v>33</v>
       </c>
       <c r="X5" s="60"/>
-      <c r="Y5" s="118"/>
+      <c r="Y5" s="142"/>
       <c r="Z5" s="72" t="s">
         <v>70</v>
       </c>
@@ -2194,9 +2200,9 @@
       </c>
       <c r="AB5" s="74"/>
       <c r="AC5" s="75"/>
-      <c r="AE5" s="117"/>
-      <c r="AF5" s="117"/>
-      <c r="AG5" s="117"/>
+      <c r="AE5" s="125"/>
+      <c r="AF5" s="125"/>
+      <c r="AG5" s="125"/>
     </row>
     <row r="6" spans="2:33" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="39" t="s">
@@ -2215,9 +2221,9 @@
       <c r="I6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="119"/>
-      <c r="K6" s="120"/>
-      <c r="L6" s="120"/>
+      <c r="J6" s="132"/>
+      <c r="K6" s="133"/>
+      <c r="L6" s="133"/>
       <c r="M6" s="14"/>
       <c r="N6" s="99" t="s">
         <v>77</v>
@@ -2231,7 +2237,7 @@
       <c r="R6" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="S6" s="116"/>
+      <c r="S6" s="140"/>
       <c r="T6" s="64"/>
       <c r="U6" s="26" t="s">
         <v>16</v>
@@ -2243,7 +2249,7 @@
         <v>31</v>
       </c>
       <c r="X6" s="60"/>
-      <c r="Y6" s="118"/>
+      <c r="Y6" s="142"/>
       <c r="Z6" s="76"/>
       <c r="AA6" s="77"/>
       <c r="AB6" s="78" t="s">
@@ -2252,9 +2258,9 @@
       <c r="AC6" s="79" t="s">
         <v>70</v>
       </c>
-      <c r="AE6" s="117"/>
-      <c r="AF6" s="117"/>
-      <c r="AG6" s="117"/>
+      <c r="AE6" s="125"/>
+      <c r="AF6" s="125"/>
+      <c r="AG6" s="125"/>
     </row>
     <row r="7" spans="2:33" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="33" t="s">
@@ -2263,11 +2269,11 @@
       <c r="C7" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="119" t="s">
+      <c r="D7" s="132" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="120"/>
-      <c r="F7" s="120"/>
+      <c r="E7" s="133"/>
+      <c r="F7" s="133"/>
       <c r="G7" s="94"/>
       <c r="H7" s="5" t="s">
         <v>15</v>
@@ -2275,9 +2281,9 @@
       <c r="I7" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="119"/>
-      <c r="K7" s="120"/>
-      <c r="L7" s="120"/>
+      <c r="J7" s="132"/>
+      <c r="K7" s="133"/>
+      <c r="L7" s="133"/>
       <c r="M7" s="14"/>
       <c r="N7" s="28" t="s">
         <v>8</v>
@@ -2291,7 +2297,7 @@
       <c r="R7" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="S7" s="116"/>
+      <c r="S7" s="140"/>
       <c r="T7" s="64"/>
       <c r="U7" s="30" t="s">
         <v>6</v>
@@ -2303,7 +2309,7 @@
         <v>27</v>
       </c>
       <c r="X7" s="60"/>
-      <c r="Y7" s="118"/>
+      <c r="Y7" s="142"/>
       <c r="Z7" s="80"/>
       <c r="AA7" s="81"/>
       <c r="AB7" s="82" t="s">
@@ -2312,9 +2318,9 @@
       <c r="AC7" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="AE7" s="117"/>
-      <c r="AF7" s="117"/>
-      <c r="AG7" s="117"/>
+      <c r="AE7" s="125"/>
+      <c r="AF7" s="125"/>
+      <c r="AG7" s="125"/>
     </row>
     <row r="8" spans="2:33" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="39" t="s">
@@ -2323,21 +2329,21 @@
       <c r="C8" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="119"/>
-      <c r="E8" s="120"/>
-      <c r="F8" s="120"/>
+      <c r="D8" s="132"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="133"/>
       <c r="G8" s="67"/>
       <c r="H8" s="11" t="s">
         <v>14</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="J8" s="121" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="134" t="s">
         <v>43</v>
       </c>
-      <c r="K8" s="122"/>
-      <c r="L8" s="122"/>
+      <c r="K8" s="135"/>
+      <c r="L8" s="135"/>
       <c r="M8" s="2"/>
       <c r="N8" s="24" t="s">
         <v>16</v>
@@ -2346,12 +2352,12 @@
         <v>25</v>
       </c>
       <c r="Q8" s="22" t="s">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="R8" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="S8" s="116"/>
+      <c r="S8" s="140"/>
       <c r="T8" s="64"/>
       <c r="U8" s="26" t="s">
         <v>14</v>
@@ -2363,14 +2369,14 @@
         <v>20</v>
       </c>
       <c r="X8" s="60"/>
-      <c r="Y8" s="118"/>
+      <c r="Y8" s="142"/>
       <c r="Z8" s="3"/>
       <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
       <c r="AC8" s="3"/>
-      <c r="AE8" s="117"/>
-      <c r="AF8" s="117"/>
-      <c r="AG8" s="117"/>
+      <c r="AE8" s="125"/>
+      <c r="AF8" s="125"/>
+      <c r="AG8" s="125"/>
     </row>
     <row r="9" spans="2:33" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="33" t="s">
@@ -2379,9 +2385,9 @@
       <c r="C9" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="119"/>
-      <c r="E9" s="120"/>
-      <c r="F9" s="120"/>
+      <c r="D9" s="132"/>
+      <c r="E9" s="133"/>
+      <c r="F9" s="133"/>
       <c r="G9" s="94"/>
       <c r="H9" s="5" t="s">
         <v>18</v>
@@ -2401,7 +2407,7 @@
       <c r="R9" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="S9" s="116"/>
+      <c r="S9" s="140"/>
       <c r="T9" s="64"/>
       <c r="U9" s="30" t="s">
         <v>4</v>
@@ -2413,7 +2419,7 @@
         <v>21</v>
       </c>
       <c r="X9" s="60"/>
-      <c r="Y9" s="118"/>
+      <c r="Y9" s="142"/>
       <c r="Z9" s="68"/>
       <c r="AA9" s="69"/>
       <c r="AB9" s="70" t="s">
@@ -2422,9 +2428,9 @@
       <c r="AC9" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="AE9" s="117"/>
-      <c r="AF9" s="117"/>
-      <c r="AG9" s="117"/>
+      <c r="AE9" s="125"/>
+      <c r="AF9" s="125"/>
+      <c r="AG9" s="125"/>
     </row>
     <row r="10" spans="2:33" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="39" t="s">
@@ -2433,9 +2439,9 @@
       <c r="C10" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="119"/>
-      <c r="E10" s="120"/>
-      <c r="F10" s="120"/>
+      <c r="D10" s="132"/>
+      <c r="E10" s="133"/>
+      <c r="F10" s="133"/>
       <c r="G10" s="94"/>
       <c r="H10" s="11" t="s">
         <v>13</v>
@@ -2443,16 +2449,16 @@
       <c r="I10" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J10" s="119" t="s">
+      <c r="J10" s="132" t="s">
         <v>57</v>
       </c>
-      <c r="K10" s="120"/>
-      <c r="L10" s="120"/>
+      <c r="K10" s="133"/>
+      <c r="L10" s="133"/>
       <c r="N10" s="24" t="s">
         <v>14</v>
       </c>
       <c r="O10" s="30" t="s">
-        <v>78</v>
+        <v>22</v>
       </c>
       <c r="Q10" s="22" t="s">
         <v>5</v>
@@ -2460,7 +2466,7 @@
       <c r="R10" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="S10" s="116"/>
+      <c r="S10" s="140"/>
       <c r="T10" s="64"/>
       <c r="U10" s="26" t="s">
         <v>13</v>
@@ -2472,7 +2478,7 @@
         <v>29</v>
       </c>
       <c r="X10" s="60"/>
-      <c r="Y10" s="118"/>
+      <c r="Y10" s="142"/>
       <c r="Z10" s="72"/>
       <c r="AA10" s="73"/>
       <c r="AB10" s="74" t="s">
@@ -2481,9 +2487,9 @@
       <c r="AC10" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="AE10" s="117"/>
-      <c r="AF10" s="117"/>
-      <c r="AG10" s="117"/>
+      <c r="AE10" s="125"/>
+      <c r="AF10" s="125"/>
+      <c r="AG10" s="125"/>
     </row>
     <row r="11" spans="2:33" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="33" t="s">
@@ -2492,9 +2498,9 @@
       <c r="C11" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="119"/>
-      <c r="E11" s="120"/>
-      <c r="F11" s="120"/>
+      <c r="D11" s="132"/>
+      <c r="E11" s="133"/>
+      <c r="F11" s="133"/>
       <c r="G11" s="94"/>
       <c r="H11" s="5" t="s">
         <v>12</v>
@@ -2502,9 +2508,9 @@
       <c r="I11" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="J11" s="119"/>
-      <c r="K11" s="120"/>
-      <c r="L11" s="120"/>
+      <c r="J11" s="132"/>
+      <c r="K11" s="133"/>
+      <c r="L11" s="133"/>
       <c r="N11" s="28" t="s">
         <v>4</v>
       </c>
@@ -2517,7 +2523,7 @@
       <c r="R11" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="S11" s="116"/>
+      <c r="S11" s="140"/>
       <c r="T11" s="64"/>
       <c r="U11" s="30" t="s">
         <v>2</v>
@@ -2527,7 +2533,7 @@
         <v>30</v>
       </c>
       <c r="X11" s="60"/>
-      <c r="Y11" s="118"/>
+      <c r="Y11" s="142"/>
       <c r="Z11" s="76" t="s">
         <v>70</v>
       </c>
@@ -2536,9 +2542,9 @@
       </c>
       <c r="AB11" s="78"/>
       <c r="AC11" s="79"/>
-      <c r="AE11" s="117"/>
-      <c r="AF11" s="117"/>
-      <c r="AG11" s="117"/>
+      <c r="AE11" s="125"/>
+      <c r="AF11" s="125"/>
+      <c r="AG11" s="125"/>
     </row>
     <row r="12" spans="2:33" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="39" t="s">
@@ -2547,9 +2553,9 @@
       <c r="C12" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="119"/>
-      <c r="E12" s="120"/>
-      <c r="F12" s="120"/>
+      <c r="D12" s="132"/>
+      <c r="E12" s="133"/>
+      <c r="F12" s="133"/>
       <c r="G12" s="94"/>
       <c r="H12" s="11" t="s">
         <v>11</v>
@@ -2557,9 +2563,9 @@
       <c r="I12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="J12" s="119"/>
-      <c r="K12" s="120"/>
-      <c r="L12" s="120"/>
+      <c r="J12" s="132"/>
+      <c r="K12" s="133"/>
+      <c r="L12" s="133"/>
       <c r="N12" s="24" t="s">
         <v>13</v>
       </c>
@@ -2572,7 +2578,7 @@
       <c r="R12" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="S12" s="116"/>
+      <c r="S12" s="140"/>
       <c r="T12" s="64"/>
       <c r="U12" s="26" t="s">
         <v>11</v>
@@ -2584,7 +2590,7 @@
         <v>26</v>
       </c>
       <c r="X12" s="60"/>
-      <c r="Y12" s="118"/>
+      <c r="Y12" s="142"/>
       <c r="Z12" s="80" t="s">
         <v>37</v>
       </c>
@@ -2604,9 +2610,9 @@
       <c r="C13" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="119"/>
-      <c r="E13" s="120"/>
-      <c r="F13" s="120"/>
+      <c r="D13" s="132"/>
+      <c r="E13" s="133"/>
+      <c r="F13" s="133"/>
       <c r="G13" s="94"/>
       <c r="H13" s="5" t="s">
         <v>10</v>
@@ -2614,9 +2620,9 @@
       <c r="I13" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="J13" s="119"/>
-      <c r="K13" s="120"/>
-      <c r="L13" s="120"/>
+      <c r="J13" s="132"/>
+      <c r="K13" s="133"/>
+      <c r="L13" s="133"/>
       <c r="N13" s="28" t="s">
         <v>2</v>
       </c>
@@ -2629,7 +2635,7 @@
       <c r="R13" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="S13" s="116"/>
+      <c r="S13" s="140"/>
       <c r="T13" s="64"/>
       <c r="U13" s="43" t="s">
         <v>0</v>
@@ -2639,7 +2645,7 @@
         <v>35</v>
       </c>
       <c r="X13" s="60"/>
-      <c r="Y13" s="118"/>
+      <c r="Y13" s="142"/>
       <c r="Z13" s="3"/>
       <c r="AA13" s="3"/>
       <c r="AB13" s="3"/>
@@ -2655,9 +2661,9 @@
       <c r="C14" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="119"/>
-      <c r="E14" s="120"/>
-      <c r="F14" s="120"/>
+      <c r="D14" s="132"/>
+      <c r="E14" s="133"/>
+      <c r="F14" s="133"/>
       <c r="G14" s="94"/>
       <c r="H14" s="11" t="s">
         <v>9</v>
@@ -2665,9 +2671,9 @@
       <c r="I14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="119"/>
-      <c r="K14" s="120"/>
-      <c r="L14" s="120"/>
+      <c r="J14" s="132"/>
+      <c r="K14" s="133"/>
+      <c r="L14" s="133"/>
       <c r="N14" s="24" t="s">
         <v>11</v>
       </c>
@@ -2680,13 +2686,13 @@
       <c r="R14" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="S14" s="116"/>
+      <c r="S14" s="140"/>
       <c r="T14" s="65"/>
       <c r="U14" s="58"/>
       <c r="V14" s="57"/>
       <c r="W14" s="56"/>
       <c r="X14" s="61"/>
-      <c r="Y14" s="118"/>
+      <c r="Y14" s="142"/>
       <c r="Z14" s="68" t="s">
         <v>37</v>
       </c>
@@ -2695,11 +2701,11 @@
       </c>
       <c r="AB14" s="85"/>
       <c r="AC14" s="71"/>
-      <c r="AE14" s="117" t="s">
+      <c r="AE14" s="125" t="s">
         <v>69</v>
       </c>
-      <c r="AF14" s="117"/>
-      <c r="AG14" s="117"/>
+      <c r="AF14" s="125"/>
+      <c r="AG14" s="125"/>
     </row>
     <row r="15" spans="2:33" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="33" t="s">
@@ -2708,9 +2714,9 @@
       <c r="C15" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="119"/>
-      <c r="E15" s="120"/>
-      <c r="F15" s="120"/>
+      <c r="D15" s="132"/>
+      <c r="E15" s="133"/>
+      <c r="F15" s="133"/>
       <c r="G15" s="94"/>
       <c r="H15" s="5" t="s">
         <v>8</v>
@@ -2718,14 +2724,14 @@
       <c r="I15" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="119"/>
-      <c r="K15" s="120"/>
-      <c r="L15" s="120"/>
+      <c r="J15" s="132"/>
+      <c r="K15" s="133"/>
+      <c r="L15" s="133"/>
       <c r="N15" s="29" t="s">
         <v>0</v>
       </c>
       <c r="O15" s="27" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="Q15" s="18" t="s">
         <v>10</v>
@@ -2733,13 +2739,13 @@
       <c r="R15" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="S15" s="116"/>
+      <c r="S15" s="140"/>
       <c r="T15" s="64"/>
       <c r="U15" s="55"/>
       <c r="V15" s="53"/>
       <c r="W15" s="54"/>
       <c r="X15" s="60"/>
-      <c r="Y15" s="118"/>
+      <c r="Y15" s="142"/>
       <c r="Z15" s="72" t="s">
         <v>70</v>
       </c>
@@ -2748,9 +2754,9 @@
       </c>
       <c r="AB15" s="77"/>
       <c r="AC15" s="75"/>
-      <c r="AE15" s="117"/>
-      <c r="AF15" s="117"/>
-      <c r="AG15" s="117"/>
+      <c r="AE15" s="125"/>
+      <c r="AF15" s="125"/>
+      <c r="AG15" s="125"/>
     </row>
     <row r="16" spans="2:33" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="39" t="s">
@@ -2759,20 +2765,20 @@
       <c r="C16" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="119"/>
-      <c r="E16" s="120"/>
-      <c r="F16" s="120"/>
+      <c r="D16" s="132"/>
+      <c r="E16" s="133"/>
+      <c r="F16" s="133"/>
       <c r="G16" s="94"/>
       <c r="H16" s="11" t="s">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="J16" s="119"/>
-      <c r="K16" s="120"/>
-      <c r="L16" s="120"/>
-      <c r="S16" s="116"/>
+      <c r="J16" s="132"/>
+      <c r="K16" s="133"/>
+      <c r="L16" s="133"/>
+      <c r="S16" s="140"/>
       <c r="T16" s="64"/>
       <c r="U16" s="44" t="s">
         <v>9</v>
@@ -2782,7 +2788,7 @@
         <v>23</v>
       </c>
       <c r="X16" s="60"/>
-      <c r="Y16" s="118"/>
+      <c r="Y16" s="142"/>
       <c r="Z16" s="76"/>
       <c r="AA16" s="74"/>
       <c r="AB16" s="87" t="s">
@@ -2791,9 +2797,9 @@
       <c r="AC16" s="79" t="s">
         <v>70</v>
       </c>
-      <c r="AE16" s="117"/>
-      <c r="AF16" s="117"/>
-      <c r="AG16" s="117"/>
+      <c r="AE16" s="125"/>
+      <c r="AF16" s="125"/>
+      <c r="AG16" s="125"/>
     </row>
     <row r="17" spans="2:33" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B17" s="33" t="s">
@@ -2802,9 +2808,9 @@
       <c r="C17" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="119"/>
-      <c r="E17" s="120"/>
-      <c r="F17" s="120"/>
+      <c r="D17" s="132"/>
+      <c r="E17" s="133"/>
+      <c r="F17" s="133"/>
       <c r="G17" s="94"/>
       <c r="H17" s="5" t="s">
         <v>6</v>
@@ -2812,17 +2818,17 @@
       <c r="I17" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="J17" s="119"/>
-      <c r="K17" s="120"/>
-      <c r="L17" s="120"/>
-      <c r="N17" s="117" t="s">
+      <c r="J17" s="132"/>
+      <c r="K17" s="133"/>
+      <c r="L17" s="133"/>
+      <c r="N17" s="125" t="s">
         <v>67</v>
       </c>
-      <c r="O17" s="117"/>
-      <c r="P17" s="117"/>
-      <c r="Q17" s="117"/>
-      <c r="R17" s="117"/>
-      <c r="S17" s="116"/>
+      <c r="O17" s="125"/>
+      <c r="P17" s="125"/>
+      <c r="Q17" s="125"/>
+      <c r="R17" s="125"/>
+      <c r="S17" s="140"/>
       <c r="T17" s="64"/>
       <c r="U17" s="17" t="s">
         <v>17</v>
@@ -2834,7 +2840,7 @@
         <v>24</v>
       </c>
       <c r="X17" s="60"/>
-      <c r="Y17" s="118"/>
+      <c r="Y17" s="142"/>
       <c r="Z17" s="80"/>
       <c r="AA17" s="88"/>
       <c r="AB17" s="89" t="s">
@@ -2843,9 +2849,9 @@
       <c r="AC17" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="AE17" s="117"/>
-      <c r="AF17" s="117"/>
-      <c r="AG17" s="117"/>
+      <c r="AE17" s="125"/>
+      <c r="AF17" s="125"/>
+      <c r="AG17" s="125"/>
     </row>
     <row r="18" spans="2:33" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="39" t="s">
@@ -2854,9 +2860,9 @@
       <c r="C18" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="119"/>
-      <c r="E18" s="120"/>
-      <c r="F18" s="120"/>
+      <c r="D18" s="132"/>
+      <c r="E18" s="133"/>
+      <c r="F18" s="133"/>
       <c r="G18" s="94"/>
       <c r="H18" s="11" t="s">
         <v>5</v>
@@ -2864,18 +2870,18 @@
       <c r="I18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J18" s="119"/>
-      <c r="K18" s="120"/>
-      <c r="L18" s="120"/>
-      <c r="N18" s="117"/>
-      <c r="O18" s="117"/>
-      <c r="P18" s="117"/>
-      <c r="Q18" s="117"/>
-      <c r="R18" s="117"/>
-      <c r="S18" s="116"/>
+      <c r="J18" s="132"/>
+      <c r="K18" s="133"/>
+      <c r="L18" s="133"/>
+      <c r="N18" s="125"/>
+      <c r="O18" s="125"/>
+      <c r="P18" s="125"/>
+      <c r="Q18" s="125"/>
+      <c r="R18" s="125"/>
+      <c r="S18" s="140"/>
       <c r="T18" s="64"/>
       <c r="U18" s="21" t="s">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="V18" s="106" t="s">
         <v>72</v>
@@ -2884,14 +2890,14 @@
         <v>25</v>
       </c>
       <c r="X18" s="60"/>
-      <c r="Y18" s="118"/>
+      <c r="Y18" s="142"/>
       <c r="Z18" s="3"/>
       <c r="AA18" s="3"/>
       <c r="AB18" s="3"/>
       <c r="AC18" s="3"/>
-      <c r="AE18" s="117"/>
-      <c r="AF18" s="117"/>
-      <c r="AG18" s="117"/>
+      <c r="AE18" s="125"/>
+      <c r="AF18" s="125"/>
+      <c r="AG18" s="125"/>
     </row>
     <row r="19" spans="2:33" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="33" t="s">
@@ -2900,9 +2906,9 @@
       <c r="C19" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="119"/>
-      <c r="E19" s="120"/>
-      <c r="F19" s="120"/>
+      <c r="D19" s="132"/>
+      <c r="E19" s="133"/>
+      <c r="F19" s="133"/>
       <c r="G19" s="94"/>
       <c r="H19" s="5" t="s">
         <v>4</v>
@@ -2910,15 +2916,15 @@
       <c r="I19" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="J19" s="119"/>
-      <c r="K19" s="120"/>
-      <c r="L19" s="120"/>
-      <c r="N19" s="117"/>
-      <c r="O19" s="117"/>
-      <c r="P19" s="117"/>
-      <c r="Q19" s="117"/>
-      <c r="R19" s="117"/>
-      <c r="S19" s="116"/>
+      <c r="J19" s="132"/>
+      <c r="K19" s="133"/>
+      <c r="L19" s="133"/>
+      <c r="N19" s="125"/>
+      <c r="O19" s="125"/>
+      <c r="P19" s="125"/>
+      <c r="Q19" s="125"/>
+      <c r="R19" s="125"/>
+      <c r="S19" s="140"/>
       <c r="T19" s="64"/>
       <c r="U19" s="17" t="s">
         <v>15</v>
@@ -2930,7 +2936,7 @@
         <v>41</v>
       </c>
       <c r="X19" s="60"/>
-      <c r="Y19" s="118"/>
+      <c r="Y19" s="142"/>
       <c r="Z19" s="68"/>
       <c r="AA19" s="84"/>
       <c r="AB19" s="85" t="s">
@@ -2947,9 +2953,9 @@
       <c r="C20" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="119"/>
-      <c r="E20" s="120"/>
-      <c r="F20" s="120"/>
+      <c r="D20" s="132"/>
+      <c r="E20" s="133"/>
+      <c r="F20" s="133"/>
       <c r="G20" s="94"/>
       <c r="H20" s="11" t="s">
         <v>3</v>
@@ -2957,15 +2963,15 @@
       <c r="I20" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="J20" s="119"/>
-      <c r="K20" s="120"/>
-      <c r="L20" s="120"/>
-      <c r="N20" s="117"/>
-      <c r="O20" s="117"/>
-      <c r="P20" s="117"/>
-      <c r="Q20" s="117"/>
-      <c r="R20" s="117"/>
-      <c r="S20" s="116"/>
+      <c r="J20" s="132"/>
+      <c r="K20" s="133"/>
+      <c r="L20" s="133"/>
+      <c r="N20" s="125"/>
+      <c r="O20" s="125"/>
+      <c r="P20" s="125"/>
+      <c r="Q20" s="125"/>
+      <c r="R20" s="125"/>
+      <c r="S20" s="140"/>
       <c r="T20" s="64"/>
       <c r="U20" s="21" t="s">
         <v>5</v>
@@ -2974,10 +2980,10 @@
         <v>76</v>
       </c>
       <c r="W20" s="30" t="s">
-        <v>78</v>
+        <v>22</v>
       </c>
       <c r="X20" s="60"/>
-      <c r="Y20" s="118"/>
+      <c r="Y20" s="142"/>
       <c r="Z20" s="72"/>
       <c r="AA20" s="86"/>
       <c r="AB20" s="77" t="s">
@@ -2986,11 +2992,11 @@
       <c r="AC20" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="AE20" s="117" t="s">
+      <c r="AE20" s="125" t="s">
         <v>66</v>
       </c>
-      <c r="AF20" s="117"/>
-      <c r="AG20" s="117"/>
+      <c r="AF20" s="125"/>
+      <c r="AG20" s="125"/>
     </row>
     <row r="21" spans="2:33" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="33" t="s">
@@ -2999,9 +3005,9 @@
       <c r="C21" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="119"/>
-      <c r="E21" s="120"/>
-      <c r="F21" s="120"/>
+      <c r="D21" s="132"/>
+      <c r="E21" s="133"/>
+      <c r="F21" s="133"/>
       <c r="G21" s="94"/>
       <c r="H21" s="5" t="s">
         <v>2</v>
@@ -3009,15 +3015,15 @@
       <c r="I21" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="J21" s="119"/>
-      <c r="K21" s="120"/>
-      <c r="L21" s="120"/>
-      <c r="N21" s="117"/>
-      <c r="O21" s="117"/>
-      <c r="P21" s="117"/>
-      <c r="Q21" s="117"/>
-      <c r="R21" s="117"/>
-      <c r="S21" s="116"/>
+      <c r="J21" s="132"/>
+      <c r="K21" s="133"/>
+      <c r="L21" s="133"/>
+      <c r="N21" s="125"/>
+      <c r="O21" s="125"/>
+      <c r="P21" s="125"/>
+      <c r="Q21" s="125"/>
+      <c r="R21" s="125"/>
+      <c r="S21" s="140"/>
       <c r="T21" s="64"/>
       <c r="U21" s="17" t="s">
         <v>18</v>
@@ -3029,7 +3035,7 @@
         <v>28</v>
       </c>
       <c r="X21" s="60"/>
-      <c r="Y21" s="118"/>
+      <c r="Y21" s="142"/>
       <c r="Z21" s="76" t="s">
         <v>70</v>
       </c>
@@ -3049,9 +3055,9 @@
       <c r="C22" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="119"/>
-      <c r="E22" s="120"/>
-      <c r="F22" s="120"/>
+      <c r="D22" s="132"/>
+      <c r="E22" s="133"/>
+      <c r="F22" s="133"/>
       <c r="G22" s="94"/>
       <c r="H22" s="11" t="s">
         <v>1</v>
@@ -3059,17 +3065,17 @@
       <c r="I22" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J22" s="119"/>
-      <c r="K22" s="120"/>
-      <c r="L22" s="120"/>
-      <c r="N22" s="114" t="s">
+      <c r="J22" s="132"/>
+      <c r="K22" s="133"/>
+      <c r="L22" s="133"/>
+      <c r="N22" s="137" t="s">
         <v>46</v>
       </c>
-      <c r="O22" s="114"/>
-      <c r="P22" s="114"/>
-      <c r="Q22" s="114"/>
-      <c r="R22" s="114"/>
-      <c r="S22" s="116"/>
+      <c r="O22" s="137"/>
+      <c r="P22" s="137"/>
+      <c r="Q22" s="137"/>
+      <c r="R22" s="137"/>
+      <c r="S22" s="140"/>
       <c r="T22" s="64"/>
       <c r="U22" s="21" t="s">
         <v>3</v>
@@ -3081,7 +3087,7 @@
         <v>36</v>
       </c>
       <c r="X22" s="60"/>
-      <c r="Y22" s="118"/>
+      <c r="Y22" s="142"/>
       <c r="Z22" s="80" t="s">
         <v>37</v>
       </c>
@@ -3090,10 +3096,10 @@
       </c>
       <c r="AB22" s="89"/>
       <c r="AC22" s="83"/>
-      <c r="AE22" s="117" t="s">
+      <c r="AE22" s="125" t="s">
         <v>63</v>
       </c>
-      <c r="AF22" s="117"/>
+      <c r="AF22" s="125"/>
       <c r="AG22" s="42" t="s">
         <v>47</v>
       </c>
@@ -3105,20 +3111,20 @@
       <c r="C23" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="119"/>
-      <c r="E23" s="120"/>
-      <c r="F23" s="120"/>
+      <c r="D23" s="132"/>
+      <c r="E23" s="133"/>
+      <c r="F23" s="133"/>
       <c r="G23" s="94"/>
       <c r="H23" s="7" t="s">
         <v>0</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="J23" s="119"/>
-      <c r="K23" s="120"/>
-      <c r="L23" s="120"/>
-      <c r="S23" s="116"/>
+        <v>83</v>
+      </c>
+      <c r="J23" s="132"/>
+      <c r="K23" s="133"/>
+      <c r="L23" s="133"/>
+      <c r="S23" s="140"/>
       <c r="T23" s="64"/>
       <c r="U23" s="17" t="s">
         <v>12</v>
@@ -3128,16 +3134,16 @@
         <v>34</v>
       </c>
       <c r="X23" s="60"/>
-      <c r="Y23" s="118"/>
+      <c r="Y23" s="142"/>
       <c r="Z23" s="90"/>
       <c r="AA23" s="90"/>
       <c r="AB23" s="90"/>
       <c r="AC23" s="90"/>
       <c r="AD23" s="90"/>
-      <c r="AE23" s="117" t="s">
+      <c r="AE23" s="125" t="s">
         <v>64</v>
       </c>
-      <c r="AF23" s="117"/>
+      <c r="AF23" s="125"/>
       <c r="AG23" s="42" t="s">
         <v>47</v>
       </c>
@@ -3149,15 +3155,15 @@
       <c r="N24" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="O24" s="127" t="s">
+      <c r="O24" s="126" t="s">
         <v>54</v>
       </c>
-      <c r="P24" s="129"/>
-      <c r="Q24" s="127" t="s">
+      <c r="P24" s="128"/>
+      <c r="Q24" s="126" t="s">
         <v>55</v>
       </c>
-      <c r="R24" s="128"/>
-      <c r="S24" s="116"/>
+      <c r="R24" s="127"/>
+      <c r="S24" s="140"/>
       <c r="T24" s="64"/>
       <c r="U24" s="21" t="s">
         <v>1</v>
@@ -3169,16 +3175,16 @@
         <v>32</v>
       </c>
       <c r="X24" s="60"/>
-      <c r="Y24" s="118"/>
+      <c r="Y24" s="142"/>
       <c r="Z24" s="90"/>
       <c r="AA24" s="90"/>
       <c r="AB24" s="90"/>
       <c r="AC24" s="90"/>
       <c r="AD24" s="90"/>
-      <c r="AE24" s="117" t="s">
+      <c r="AE24" s="125" t="s">
         <v>65</v>
       </c>
-      <c r="AF24" s="117"/>
+      <c r="AF24" s="125"/>
       <c r="AG24" s="42" t="s">
         <v>47</v>
       </c>
@@ -3197,25 +3203,25 @@
       <c r="N25" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="O25" s="130">
+      <c r="O25" s="129">
         <v>0.8</v>
       </c>
-      <c r="P25" s="131"/>
-      <c r="Q25" s="130">
+      <c r="P25" s="130"/>
+      <c r="Q25" s="129">
         <v>100</v>
       </c>
-      <c r="R25" s="132"/>
-      <c r="S25" s="116"/>
+      <c r="R25" s="131"/>
+      <c r="S25" s="140"/>
       <c r="T25" s="66"/>
       <c r="U25" s="19" t="s">
         <v>10</v>
       </c>
       <c r="V25" s="53"/>
       <c r="W25" s="27" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="X25" s="62"/>
-      <c r="Y25" s="118"/>
+      <c r="Y25" s="142"/>
       <c r="Z25" s="90"/>
       <c r="AA25" s="90"/>
       <c r="AB25" s="90"/>
@@ -3239,21 +3245,21 @@
       <c r="N26" s="96" t="s">
         <v>59</v>
       </c>
-      <c r="O26" s="123">
+      <c r="O26" s="121">
         <v>1</v>
       </c>
-      <c r="P26" s="124"/>
-      <c r="Q26" s="123">
+      <c r="P26" s="122"/>
+      <c r="Q26" s="121">
         <v>180</v>
       </c>
-      <c r="R26" s="126"/>
-      <c r="S26" s="116"/>
+      <c r="R26" s="124"/>
+      <c r="S26" s="140"/>
       <c r="T26" s="47"/>
       <c r="U26" s="50"/>
       <c r="V26" s="51"/>
       <c r="W26" s="52"/>
       <c r="X26" s="47"/>
-      <c r="Y26" s="118"/>
+      <c r="Y26" s="142"/>
       <c r="Z26" s="91"/>
       <c r="AA26" s="91"/>
       <c r="AB26" s="91"/>
@@ -3274,18 +3280,18 @@
       <c r="J27" s="98"/>
       <c r="K27" s="98"/>
       <c r="L27" s="98"/>
-      <c r="N27" s="125" t="s">
+      <c r="N27" s="123" t="s">
         <v>60</v>
       </c>
-      <c r="O27" s="125"/>
-      <c r="P27" s="125"/>
-      <c r="Q27" s="125"/>
-      <c r="R27" s="125"/>
-      <c r="U27" s="113" t="s">
+      <c r="O27" s="123"/>
+      <c r="P27" s="123"/>
+      <c r="Q27" s="123"/>
+      <c r="R27" s="123"/>
+      <c r="U27" s="136" t="s">
         <v>52</v>
       </c>
-      <c r="V27" s="114"/>
-      <c r="W27" s="114"/>
+      <c r="V27" s="137"/>
+      <c r="W27" s="137"/>
       <c r="Z27" s="91"/>
       <c r="AA27" s="91"/>
       <c r="AB27" s="91"/>
@@ -3301,14 +3307,14 @@
       <c r="AG28" s="91"/>
     </row>
     <row r="29" spans="2:33" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N29" s="113" t="s">
+      <c r="N29" s="136" t="s">
         <v>61</v>
       </c>
-      <c r="O29" s="114"/>
-      <c r="Q29" s="115" t="s">
+      <c r="O29" s="137"/>
+      <c r="Q29" s="138" t="s">
         <v>62</v>
       </c>
-      <c r="R29" s="115"/>
+      <c r="R29" s="138"/>
     </row>
     <row r="30" spans="2:33" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="N30" s="108" t="s">
@@ -3325,16 +3331,16 @@
       </c>
     </row>
     <row r="31" spans="2:33" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N31" s="138" t="s">
+      <c r="N31" s="118" t="s">
         <v>44</v>
       </c>
-      <c r="O31" s="137" t="s">
+      <c r="O31" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="Q31" s="139" t="s">
+      <c r="Q31" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="R31" s="140" t="s">
+      <c r="R31" s="120" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3374,7 +3380,7 @@
         <v>31</v>
       </c>
       <c r="Q34" s="39" t="s">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="R34" s="34" t="s">
         <v>25</v>
@@ -3475,25 +3481,11 @@
         <v>10</v>
       </c>
       <c r="R41" s="41" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="N27:R27"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="AE24:AF24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="D3:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D7:F23"/>
-    <mergeCell ref="J3:L7"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="J10:L23"/>
     <mergeCell ref="N29:O29"/>
     <mergeCell ref="Q29:R29"/>
     <mergeCell ref="S3:S26"/>
@@ -3510,6 +3502,20 @@
     <mergeCell ref="AE20:AG20"/>
     <mergeCell ref="AE23:AF23"/>
     <mergeCell ref="AE22:AF22"/>
+    <mergeCell ref="D3:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D7:F23"/>
+    <mergeCell ref="J3:L7"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="J10:L23"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="N27:R27"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="AE24:AF24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="Q25:R25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>